<commit_message>
hagyd így pls holnap megbeszéljük
</commit_message>
<xml_diff>
--- a/Tablazat.xlsx
+++ b/Tablazat.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balazs\OneDrive\Asztali gép\cipobolt\csukabot\csukabot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomi\Documents\GitHub\csukabot\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E98D5D6-8E28-4D38-A1E6-C1CFA2D12993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>Név</t>
   </si>
@@ -116,13 +117,22 @@
     <t>Képek leírásának elkészítése</t>
   </si>
   <si>
-    <t>Google keresés és képek</t>
+    <t>Bakancs oldal</t>
+  </si>
+  <si>
+    <t>Bakancs oldal készítése</t>
+  </si>
+  <si>
+    <t>Minden</t>
+  </si>
+  <si>
+    <t>itt volt minden teso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/\ m/\ d\.\ h:mm;@"/>
   </numFmts>
@@ -341,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -364,8 +374,6 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -679,11 +687,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,11 +800,21 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9"/>
+      <c r="B6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="18">
+        <v>45083.916666666664</v>
+      </c>
+      <c r="D6" s="18">
+        <v>45083.9375</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
@@ -882,7 +900,7 @@
       <c r="C15" s="18">
         <v>45083.819444444445</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="15" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="8" t="s">
@@ -895,80 +913,80 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
       <c r="E16" s="8"/>
       <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
       <c r="E17" s="8"/>
       <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
       <c r="E18" s="8"/>
       <c r="F18" s="9"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
       <c r="E19" s="8"/>
       <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
       <c r="E20" s="8"/>
       <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
       <c r="E21" s="8"/>
       <c r="F21" s="9"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
       <c r="E22" s="8"/>
       <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
       <c r="E23" s="8"/>
       <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
       <c r="E24" s="8"/>
       <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
       <c r="E25" s="11"/>
       <c r="F25" s="12"/>
     </row>
@@ -1012,21 +1030,11 @@
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
-      <c r="B28" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="18">
-        <v>45085.833333333336</v>
-      </c>
-      <c r="D28" s="18">
-        <v>45085.875</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
@@ -1122,11 +1130,21 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="9"/>
+      <c r="B39" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="18">
+        <v>45084.75</v>
+      </c>
+      <c r="D39" s="18">
+        <v>45084.791666666664</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>

</xml_diff>